<commit_message>
Fixed result export and single-country exception for car-sharing.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_2.xlsx
+++ b/RECC_Config_V2_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="9" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RECC_R32IND" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -752,8 +752,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -948,7 +948,7 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView topLeftCell="A115" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
@@ -967,8 +967,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5897,7 +5897,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6027,7 +6027,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -6431,8 +6431,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -11315,7 +11315,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -11361,7 +11361,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -11468,7 +11468,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -11491,7 +11491,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -11514,7 +11514,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -11537,7 +11537,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -11895,8 +11895,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -16779,7 +16779,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -16802,7 +16802,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -16825,7 +16825,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -16932,7 +16932,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -16955,7 +16955,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -16978,7 +16978,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -17001,7 +17001,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -17359,8 +17359,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -22243,7 +22243,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -22266,7 +22266,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -22289,7 +22289,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -22396,7 +22396,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -22419,7 +22419,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -22442,7 +22442,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -22465,7 +22465,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -27706,8 +27706,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="B101" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -27725,8 +27725,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -32591,7 +32591,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -32614,7 +32614,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -32637,7 +32637,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -32660,7 +32660,7 @@
       </c>
       <c r="D135" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -32688,7 +32688,7 @@
       </c>
       <c r="D136" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -32716,7 +32716,7 @@
       </c>
       <c r="D137" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E137" s="82" t="inlineStr">
@@ -32744,7 +32744,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -32767,7 +32767,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -32790,7 +32790,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -32813,7 +32813,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -32869,7 +32869,7 @@
       </c>
       <c r="D143" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E143" s="82" t="inlineStr">
@@ -32897,7 +32897,7 @@
       </c>
       <c r="D144" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E144" s="82" t="inlineStr">
@@ -33171,8 +33171,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -38635,8 +38635,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -43519,7 +43519,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -43542,7 +43542,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -43565,7 +43565,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -43672,7 +43672,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -43695,7 +43695,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -43718,7 +43718,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -43741,7 +43741,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -44099,8 +44099,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -49052,7 +49052,7 @@
       </c>
       <c r="D135" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -49080,7 +49080,7 @@
       </c>
       <c r="D136" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -49108,7 +49108,7 @@
       </c>
       <c r="D137" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E137" s="82" t="inlineStr">
@@ -49261,7 +49261,7 @@
       </c>
       <c r="D143" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E143" s="82" t="inlineStr">
@@ -49289,7 +49289,7 @@
       </c>
       <c r="D144" s="71" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E144" s="82" t="inlineStr">
@@ -49564,8 +49564,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -54448,7 +54448,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -54471,7 +54471,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -54494,7 +54494,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -54601,7 +54601,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -54624,7 +54624,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -54647,7 +54647,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -54670,7 +54670,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -55028,8 +55028,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -59912,7 +59912,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -59935,7 +59935,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -59958,7 +59958,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -60065,7 +60065,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -60088,7 +60088,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -60111,7 +60111,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -60134,7 +60134,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -60473,8 +60473,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0" zoomScale="55" zoomScaleNormal="55">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A105" workbookViewId="0" zoomScale="109" zoomScaleNormal="109">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -60492,8 +60492,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="45" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="46" style="74" width="10.6640625"/>
+    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -65376,7 +65376,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -65399,7 +65399,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -65422,7 +65422,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -65529,7 +65529,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -65552,7 +65552,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -65575,7 +65575,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -65598,7 +65598,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -65654,7 +65654,7 @@
       </c>
       <c r="D143" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E143" s="82" t="inlineStr">
@@ -65682,7 +65682,7 @@
       </c>
       <c r="D144" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E144" s="82" t="inlineStr">

</xml_diff>

<commit_message>
Lasted IRP report changes: New scenario list including USA sensitivity.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_2.xlsx
+++ b/RECC_Config_V2_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="9" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RECC_R32IND" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -326,7 +326,7 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -473,6 +473,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="1"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -750,10 +754,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B21:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -804,7 +808,7 @@
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="69" t="inlineStr">
         <is>
-          <t>RECC_EU28</t>
+          <t>RECC_R32USA</t>
         </is>
       </c>
       <c r="G4" s="26" t="n"/>
@@ -862,77 +866,653 @@
       <c r="B13" s="9" t="n"/>
       <c r="C13" s="9" t="n"/>
       <c r="D13" s="9" t="n"/>
+      <c r="E13" s="83" t="n"/>
+      <c r="F13" s="83" t="n"/>
+      <c r="G13" s="83" t="n"/>
+      <c r="H13" s="83" t="n"/>
+      <c r="I13" s="83" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="7" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="9" t="n"/>
       <c r="D14" s="9" t="n"/>
+      <c r="E14" s="83" t="n"/>
+      <c r="F14" s="83" t="n"/>
+      <c r="G14" s="83" t="n"/>
+      <c r="H14" s="83" t="n"/>
+      <c r="I14" s="83" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="7" t="n"/>
       <c r="C15" s="9" t="n"/>
       <c r="D15" s="9" t="n"/>
+      <c r="E15" s="83" t="n"/>
+      <c r="F15" s="83" t="n"/>
+      <c r="G15" s="83" t="n"/>
+      <c r="H15" s="83" t="n"/>
+      <c r="I15" s="83" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="7" t="n"/>
       <c r="B16" s="9" t="n"/>
       <c r="C16" s="9" t="n"/>
       <c r="D16" s="9" t="n"/>
+      <c r="E16" s="83" t="n"/>
+      <c r="F16" s="83" t="n"/>
+      <c r="G16" s="83" t="n"/>
+      <c r="H16" s="83" t="n"/>
+      <c r="I16" s="83" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n"/>
       <c r="C17" s="9" t="n"/>
       <c r="D17" s="9" t="n"/>
+      <c r="E17" s="83" t="n"/>
+      <c r="F17" s="83" t="n"/>
+      <c r="G17" s="83" t="n"/>
+      <c r="H17" s="83" t="n"/>
+      <c r="I17" s="83" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="n"/>
       <c r="B18" s="9" t="n"/>
       <c r="C18" s="9" t="n"/>
       <c r="D18" s="9" t="n"/>
+      <c r="E18" s="83" t="n"/>
+      <c r="F18" s="83" t="n"/>
+      <c r="G18" s="83" t="n"/>
+      <c r="H18" s="83" t="n"/>
+      <c r="I18" s="83" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n"/>
       <c r="B19" s="9" t="n"/>
       <c r="C19" s="9" t="n"/>
       <c r="D19" s="9" t="n"/>
+      <c r="E19" s="83" t="n"/>
+      <c r="F19" s="83" t="n"/>
+      <c r="G19" s="83" t="n"/>
+      <c r="H19" s="83" t="n"/>
+      <c r="I19" s="83" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="n"/>
       <c r="C20" s="9" t="n"/>
       <c r="D20" s="9" t="n"/>
+      <c r="E20" s="83" t="n"/>
+      <c r="F20" s="83" t="n"/>
+      <c r="G20" s="83" t="n"/>
+      <c r="H20" s="83" t="n"/>
+      <c r="I20" s="83" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="7" t="n"/>
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="9" t="n"/>
+      <c r="E21" s="83" t="n"/>
+      <c r="F21" s="83" t="n"/>
+      <c r="G21" s="83" t="n"/>
+      <c r="H21" s="83" t="n"/>
+      <c r="I21" s="83" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
       <c r="C22" s="9" t="n"/>
       <c r="D22" s="9" t="n"/>
+      <c r="E22" s="83" t="n"/>
+      <c r="F22" s="83" t="n"/>
+      <c r="G22" s="83" t="n"/>
+      <c r="H22" s="83" t="n"/>
+      <c r="I22" s="83" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="7" t="n"/>
       <c r="B23" s="9" t="n"/>
       <c r="C23" s="9" t="n"/>
       <c r="D23" s="9" t="n"/>
+      <c r="E23" s="83" t="n"/>
+      <c r="F23" s="83" t="n"/>
+      <c r="G23" s="83" t="n"/>
+      <c r="H23" s="83" t="n"/>
+      <c r="I23" s="83" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="7" t="n"/>
       <c r="B24" s="9" t="n"/>
       <c r="C24" s="9" t="n"/>
       <c r="D24" s="9" t="n"/>
+      <c r="E24" s="83" t="n"/>
+      <c r="F24" s="83" t="n"/>
+      <c r="G24" s="83" t="n"/>
+      <c r="H24" s="83" t="n"/>
+      <c r="I24" s="83" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="76" t="n"/>
       <c r="B25" s="80" t="n"/>
-      <c r="C25" s="3" t="n"/>
+      <c r="C25" s="84" t="n"/>
+      <c r="D25" s="83" t="n"/>
+      <c r="E25" s="83" t="n"/>
+      <c r="F25" s="83" t="n"/>
+      <c r="G25" s="83" t="n"/>
+      <c r="H25" s="83" t="n"/>
+      <c r="I25" s="83" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="76" t="n"/>
       <c r="B26" s="80" t="n"/>
-      <c r="C26" s="3" t="n"/>
+      <c r="C26" s="84" t="n"/>
+      <c r="D26" s="83" t="n"/>
+      <c r="E26" s="83" t="n"/>
+      <c r="F26" s="83" t="n"/>
+      <c r="G26" s="83" t="n"/>
+      <c r="H26" s="83" t="n"/>
+      <c r="I26" s="83" t="n"/>
+    </row>
+    <row r="27">
+      <c r="C27" s="83" t="n"/>
+      <c r="D27" s="83" t="n"/>
+      <c r="E27" s="83" t="n"/>
+      <c r="F27" s="83" t="n"/>
+      <c r="G27" s="83" t="n"/>
+      <c r="H27" s="83" t="n"/>
+      <c r="I27" s="83" t="n"/>
+    </row>
+    <row r="28">
+      <c r="C28" s="83" t="n"/>
+      <c r="D28" s="83" t="n"/>
+      <c r="E28" s="83" t="n"/>
+      <c r="F28" s="83" t="n"/>
+      <c r="G28" s="83" t="n"/>
+      <c r="H28" s="83" t="n"/>
+      <c r="I28" s="83" t="n"/>
+    </row>
+    <row r="29">
+      <c r="C29" s="83" t="n"/>
+      <c r="D29" s="83" t="n"/>
+      <c r="E29" s="83" t="n"/>
+      <c r="F29" s="83" t="n"/>
+      <c r="G29" s="83" t="n"/>
+      <c r="H29" s="83" t="n"/>
+      <c r="I29" s="83" t="n"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="83" t="n"/>
+      <c r="D30" s="83" t="n"/>
+      <c r="E30" s="83" t="n"/>
+      <c r="F30" s="83" t="n"/>
+      <c r="G30" s="83" t="n"/>
+      <c r="H30" s="83" t="n"/>
+      <c r="I30" s="83" t="n"/>
+    </row>
+    <row r="31">
+      <c r="C31" s="83" t="n"/>
+      <c r="D31" s="83" t="n"/>
+      <c r="E31" s="83" t="n"/>
+      <c r="F31" s="83" t="n"/>
+      <c r="G31" s="83" t="n"/>
+      <c r="H31" s="83" t="n"/>
+      <c r="I31" s="83" t="n"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="83" t="n"/>
+      <c r="D32" s="83" t="n"/>
+      <c r="E32" s="83" t="n"/>
+      <c r="F32" s="83" t="n"/>
+      <c r="G32" s="83" t="n"/>
+      <c r="H32" s="83" t="n"/>
+      <c r="I32" s="83" t="n"/>
+    </row>
+    <row r="33">
+      <c r="C33" s="83" t="n"/>
+      <c r="D33" s="83" t="n"/>
+      <c r="E33" s="83" t="n"/>
+      <c r="F33" s="83" t="n"/>
+      <c r="G33" s="83" t="n"/>
+      <c r="H33" s="83" t="n"/>
+      <c r="I33" s="83" t="n"/>
+    </row>
+    <row r="34">
+      <c r="C34" s="83" t="n"/>
+      <c r="D34" s="83" t="n"/>
+      <c r="E34" s="83" t="n"/>
+      <c r="F34" s="83" t="n"/>
+      <c r="G34" s="83" t="n"/>
+      <c r="H34" s="83" t="n"/>
+      <c r="I34" s="83" t="n"/>
+    </row>
+    <row r="35">
+      <c r="C35" s="83" t="n"/>
+      <c r="D35" s="83" t="n"/>
+      <c r="E35" s="83" t="n"/>
+      <c r="F35" s="83" t="n"/>
+      <c r="G35" s="83" t="n"/>
+      <c r="H35" s="83" t="n"/>
+      <c r="I35" s="83" t="n"/>
+    </row>
+    <row r="36">
+      <c r="C36" s="83" t="n"/>
+      <c r="D36" s="83" t="n"/>
+      <c r="E36" s="83" t="n"/>
+      <c r="F36" s="83" t="n"/>
+      <c r="G36" s="83" t="n"/>
+      <c r="H36" s="83" t="n"/>
+      <c r="I36" s="83" t="n"/>
+    </row>
+    <row r="37">
+      <c r="C37" s="83" t="n"/>
+      <c r="D37" s="83" t="n"/>
+      <c r="E37" s="83" t="n"/>
+      <c r="F37" s="83" t="n"/>
+      <c r="G37" s="83" t="n"/>
+      <c r="H37" s="83" t="n"/>
+      <c r="I37" s="83" t="n"/>
+    </row>
+    <row r="38">
+      <c r="C38" s="83" t="n"/>
+      <c r="D38" s="83" t="n"/>
+      <c r="E38" s="83" t="n"/>
+      <c r="F38" s="83" t="n"/>
+      <c r="G38" s="83" t="n"/>
+      <c r="H38" s="83" t="n"/>
+      <c r="I38" s="83" t="n"/>
+    </row>
+    <row r="39">
+      <c r="C39" s="83" t="n"/>
+      <c r="D39" s="83" t="n"/>
+      <c r="E39" s="83" t="n"/>
+      <c r="F39" s="83" t="n"/>
+      <c r="G39" s="83" t="n"/>
+      <c r="H39" s="83" t="n"/>
+      <c r="I39" s="83" t="n"/>
+    </row>
+    <row r="40">
+      <c r="C40" s="83" t="n"/>
+      <c r="D40" s="83" t="n"/>
+      <c r="E40" s="83" t="n"/>
+      <c r="F40" s="83" t="n"/>
+      <c r="G40" s="83" t="n"/>
+      <c r="H40" s="83" t="n"/>
+      <c r="I40" s="83" t="n"/>
+    </row>
+    <row r="41">
+      <c r="C41" s="83" t="n"/>
+      <c r="D41" s="83" t="n"/>
+      <c r="E41" s="83" t="n"/>
+      <c r="F41" s="83" t="n"/>
+      <c r="G41" s="83" t="n"/>
+      <c r="H41" s="83" t="n"/>
+      <c r="I41" s="83" t="n"/>
+    </row>
+    <row r="42">
+      <c r="C42" s="83" t="n"/>
+      <c r="D42" s="83" t="n"/>
+      <c r="E42" s="83" t="n"/>
+      <c r="F42" s="83" t="n"/>
+      <c r="G42" s="83" t="n"/>
+      <c r="H42" s="83" t="n"/>
+      <c r="I42" s="83" t="n"/>
+    </row>
+    <row r="43">
+      <c r="C43" s="83" t="n"/>
+      <c r="D43" s="83" t="n"/>
+      <c r="E43" s="83" t="n"/>
+      <c r="F43" s="83" t="n"/>
+      <c r="G43" s="83" t="n"/>
+      <c r="H43" s="83" t="n"/>
+      <c r="I43" s="83" t="n"/>
+    </row>
+    <row r="44">
+      <c r="C44" s="83" t="n"/>
+      <c r="D44" s="83" t="n"/>
+      <c r="E44" s="83" t="n"/>
+      <c r="F44" s="83" t="n"/>
+      <c r="G44" s="83" t="n"/>
+      <c r="H44" s="83" t="n"/>
+      <c r="I44" s="83" t="n"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="83" t="n"/>
+      <c r="D45" s="83" t="n"/>
+      <c r="E45" s="83" t="n"/>
+      <c r="F45" s="83" t="n"/>
+      <c r="G45" s="83" t="n"/>
+      <c r="H45" s="83" t="n"/>
+      <c r="I45" s="83" t="n"/>
+    </row>
+    <row r="46">
+      <c r="C46" s="83" t="n"/>
+      <c r="D46" s="83" t="n"/>
+      <c r="E46" s="83" t="n"/>
+      <c r="F46" s="83" t="n"/>
+      <c r="G46" s="83" t="n"/>
+      <c r="H46" s="83" t="n"/>
+      <c r="I46" s="83" t="n"/>
+    </row>
+    <row r="47">
+      <c r="C47" s="83" t="n"/>
+      <c r="D47" s="83" t="n"/>
+      <c r="E47" s="83" t="n"/>
+      <c r="F47" s="83" t="n"/>
+      <c r="G47" s="83" t="n"/>
+      <c r="H47" s="83" t="n"/>
+      <c r="I47" s="83" t="n"/>
+    </row>
+    <row r="48">
+      <c r="C48" s="83" t="n"/>
+      <c r="D48" s="83" t="n"/>
+      <c r="E48" s="83" t="n"/>
+      <c r="F48" s="83" t="n"/>
+      <c r="G48" s="83" t="n"/>
+      <c r="H48" s="83" t="n"/>
+      <c r="I48" s="83" t="n"/>
+    </row>
+    <row r="49">
+      <c r="C49" s="83" t="n"/>
+      <c r="D49" s="83" t="n"/>
+      <c r="E49" s="83" t="n"/>
+      <c r="F49" s="83" t="n"/>
+      <c r="G49" s="83" t="n"/>
+      <c r="H49" s="83" t="n"/>
+      <c r="I49" s="83" t="n"/>
+    </row>
+    <row r="50">
+      <c r="C50" s="83" t="n"/>
+      <c r="D50" s="83" t="n"/>
+      <c r="E50" s="83" t="n"/>
+      <c r="F50" s="83" t="n"/>
+      <c r="G50" s="83" t="n"/>
+      <c r="H50" s="83" t="n"/>
+      <c r="I50" s="83" t="n"/>
+    </row>
+    <row r="51">
+      <c r="C51" s="83" t="n"/>
+      <c r="D51" s="83" t="n"/>
+      <c r="E51" s="83" t="n"/>
+      <c r="F51" s="83" t="n"/>
+      <c r="G51" s="83" t="n"/>
+      <c r="H51" s="83" t="n"/>
+      <c r="I51" s="83" t="n"/>
+    </row>
+    <row r="52">
+      <c r="C52" s="83" t="n"/>
+      <c r="D52" s="83" t="n"/>
+      <c r="E52" s="83" t="n"/>
+      <c r="F52" s="83" t="n"/>
+      <c r="G52" s="83" t="n"/>
+      <c r="H52" s="83" t="n"/>
+      <c r="I52" s="83" t="n"/>
+    </row>
+    <row r="53">
+      <c r="C53" s="83" t="n"/>
+      <c r="D53" s="83" t="n"/>
+      <c r="E53" s="83" t="n"/>
+      <c r="F53" s="83" t="n"/>
+      <c r="G53" s="83" t="n"/>
+      <c r="H53" s="83" t="n"/>
+      <c r="I53" s="83" t="n"/>
+    </row>
+    <row r="54">
+      <c r="C54" s="83" t="n"/>
+      <c r="D54" s="83" t="n"/>
+      <c r="E54" s="83" t="n"/>
+      <c r="F54" s="83" t="n"/>
+      <c r="G54" s="83" t="n"/>
+      <c r="H54" s="83" t="n"/>
+      <c r="I54" s="83" t="n"/>
+    </row>
+    <row r="55">
+      <c r="C55" s="83" t="n"/>
+      <c r="D55" s="83" t="n"/>
+      <c r="E55" s="83" t="n"/>
+      <c r="F55" s="83" t="n"/>
+      <c r="G55" s="83" t="n"/>
+      <c r="H55" s="83" t="n"/>
+      <c r="I55" s="83" t="n"/>
+    </row>
+    <row r="56">
+      <c r="C56" s="83" t="n"/>
+      <c r="D56" s="83" t="n"/>
+      <c r="E56" s="83" t="n"/>
+      <c r="F56" s="83" t="n"/>
+      <c r="G56" s="83" t="n"/>
+      <c r="H56" s="83" t="n"/>
+      <c r="I56" s="83" t="n"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="83" t="n"/>
+      <c r="D57" s="83" t="n"/>
+      <c r="E57" s="83" t="n"/>
+      <c r="F57" s="83" t="n"/>
+      <c r="G57" s="83" t="n"/>
+      <c r="H57" s="83" t="n"/>
+      <c r="I57" s="83" t="n"/>
+    </row>
+    <row r="58">
+      <c r="C58" s="83" t="n"/>
+      <c r="D58" s="83" t="n"/>
+      <c r="E58" s="83" t="n"/>
+      <c r="F58" s="83" t="n"/>
+      <c r="G58" s="83" t="n"/>
+      <c r="H58" s="83" t="n"/>
+      <c r="I58" s="83" t="n"/>
+    </row>
+    <row r="59">
+      <c r="C59" s="83" t="n"/>
+      <c r="D59" s="83" t="n"/>
+      <c r="E59" s="83" t="n"/>
+      <c r="F59" s="83" t="n"/>
+      <c r="G59" s="83" t="n"/>
+      <c r="H59" s="83" t="n"/>
+      <c r="I59" s="83" t="n"/>
+    </row>
+    <row r="60">
+      <c r="C60" s="83" t="n"/>
+      <c r="D60" s="83" t="n"/>
+      <c r="E60" s="83" t="n"/>
+      <c r="F60" s="83" t="n"/>
+      <c r="G60" s="83" t="n"/>
+      <c r="H60" s="83" t="n"/>
+      <c r="I60" s="83" t="n"/>
+    </row>
+    <row r="61">
+      <c r="C61" s="83" t="n"/>
+      <c r="D61" s="83" t="n"/>
+      <c r="E61" s="83" t="n"/>
+      <c r="F61" s="83" t="n"/>
+      <c r="G61" s="83" t="n"/>
+      <c r="H61" s="83" t="n"/>
+      <c r="I61" s="83" t="n"/>
+    </row>
+    <row r="62">
+      <c r="C62" s="83" t="n"/>
+      <c r="D62" s="83" t="n"/>
+      <c r="E62" s="83" t="n"/>
+      <c r="F62" s="83" t="n"/>
+      <c r="G62" s="83" t="n"/>
+      <c r="H62" s="83" t="n"/>
+      <c r="I62" s="83" t="n"/>
+    </row>
+    <row r="63">
+      <c r="C63" s="83" t="n"/>
+      <c r="D63" s="83" t="n"/>
+      <c r="E63" s="83" t="n"/>
+      <c r="F63" s="83" t="n"/>
+      <c r="G63" s="83" t="n"/>
+      <c r="H63" s="83" t="n"/>
+      <c r="I63" s="83" t="n"/>
+    </row>
+    <row r="64">
+      <c r="C64" s="83" t="n"/>
+      <c r="D64" s="83" t="n"/>
+      <c r="E64" s="83" t="n"/>
+      <c r="F64" s="83" t="n"/>
+      <c r="G64" s="83" t="n"/>
+      <c r="H64" s="83" t="n"/>
+      <c r="I64" s="83" t="n"/>
+    </row>
+    <row r="65">
+      <c r="C65" s="83" t="n"/>
+      <c r="D65" s="83" t="n"/>
+      <c r="E65" s="83" t="n"/>
+      <c r="F65" s="83" t="n"/>
+      <c r="G65" s="83" t="n"/>
+      <c r="H65" s="83" t="n"/>
+      <c r="I65" s="83" t="n"/>
+    </row>
+    <row r="66">
+      <c r="C66" s="83" t="n"/>
+      <c r="D66" s="83" t="n"/>
+      <c r="E66" s="83" t="n"/>
+      <c r="F66" s="83" t="n"/>
+      <c r="G66" s="83" t="n"/>
+      <c r="H66" s="83" t="n"/>
+      <c r="I66" s="83" t="n"/>
+    </row>
+    <row r="67">
+      <c r="C67" s="83" t="n"/>
+      <c r="D67" s="83" t="n"/>
+      <c r="E67" s="83" t="n"/>
+      <c r="F67" s="83" t="n"/>
+      <c r="G67" s="83" t="n"/>
+      <c r="H67" s="83" t="n"/>
+      <c r="I67" s="83" t="n"/>
+    </row>
+    <row r="68">
+      <c r="C68" s="83" t="n"/>
+      <c r="D68" s="83" t="n"/>
+      <c r="E68" s="83" t="n"/>
+      <c r="F68" s="83" t="n"/>
+      <c r="G68" s="83" t="n"/>
+      <c r="H68" s="83" t="n"/>
+      <c r="I68" s="83" t="n"/>
+    </row>
+    <row r="69">
+      <c r="C69" s="83" t="n"/>
+      <c r="D69" s="83" t="n"/>
+      <c r="E69" s="83" t="n"/>
+      <c r="F69" s="83" t="n"/>
+      <c r="G69" s="83" t="n"/>
+      <c r="H69" s="83" t="n"/>
+      <c r="I69" s="83" t="n"/>
+    </row>
+    <row r="70">
+      <c r="C70" s="83" t="n"/>
+      <c r="D70" s="83" t="n"/>
+      <c r="E70" s="83" t="n"/>
+      <c r="F70" s="83" t="n"/>
+      <c r="G70" s="83" t="n"/>
+      <c r="H70" s="83" t="n"/>
+      <c r="I70" s="83" t="n"/>
+    </row>
+    <row r="71">
+      <c r="C71" s="83" t="n"/>
+      <c r="D71" s="83" t="n"/>
+      <c r="E71" s="83" t="n"/>
+      <c r="F71" s="83" t="n"/>
+      <c r="G71" s="83" t="n"/>
+      <c r="H71" s="83" t="n"/>
+      <c r="I71" s="83" t="n"/>
+    </row>
+    <row r="72">
+      <c r="C72" s="83" t="n"/>
+      <c r="D72" s="83" t="n"/>
+      <c r="E72" s="83" t="n"/>
+      <c r="F72" s="83" t="n"/>
+      <c r="G72" s="83" t="n"/>
+      <c r="H72" s="83" t="n"/>
+      <c r="I72" s="83" t="n"/>
+    </row>
+    <row r="73">
+      <c r="C73" s="83" t="n"/>
+      <c r="D73" s="83" t="n"/>
+      <c r="E73" s="83" t="n"/>
+      <c r="F73" s="83" t="n"/>
+      <c r="G73" s="83" t="n"/>
+      <c r="H73" s="83" t="n"/>
+      <c r="I73" s="83" t="n"/>
+    </row>
+    <row r="74">
+      <c r="C74" s="83" t="n"/>
+      <c r="D74" s="83" t="n"/>
+      <c r="E74" s="83" t="n"/>
+      <c r="F74" s="83" t="n"/>
+      <c r="G74" s="83" t="n"/>
+      <c r="H74" s="83" t="n"/>
+      <c r="I74" s="83" t="n"/>
+    </row>
+    <row r="75">
+      <c r="C75" s="83" t="n"/>
+      <c r="D75" s="83" t="n"/>
+      <c r="E75" s="83" t="n"/>
+      <c r="F75" s="83" t="n"/>
+      <c r="G75" s="83" t="n"/>
+      <c r="H75" s="83" t="n"/>
+      <c r="I75" s="83" t="n"/>
+    </row>
+    <row r="76">
+      <c r="C76" s="83" t="n"/>
+      <c r="D76" s="83" t="n"/>
+      <c r="E76" s="83" t="n"/>
+      <c r="F76" s="83" t="n"/>
+      <c r="G76" s="83" t="n"/>
+      <c r="H76" s="83" t="n"/>
+      <c r="I76" s="83" t="n"/>
+    </row>
+    <row r="77">
+      <c r="C77" s="83" t="n"/>
+      <c r="D77" s="83" t="n"/>
+      <c r="E77" s="83" t="n"/>
+      <c r="F77" s="83" t="n"/>
+      <c r="G77" s="83" t="n"/>
+      <c r="H77" s="83" t="n"/>
+      <c r="I77" s="83" t="n"/>
+    </row>
+    <row r="78">
+      <c r="C78" s="83" t="n"/>
+      <c r="D78" s="83" t="n"/>
+      <c r="E78" s="83" t="n"/>
+      <c r="F78" s="83" t="n"/>
+      <c r="G78" s="83" t="n"/>
+      <c r="H78" s="83" t="n"/>
+      <c r="I78" s="83" t="n"/>
+    </row>
+    <row r="79">
+      <c r="C79" s="83" t="n"/>
+      <c r="D79" s="83" t="n"/>
+      <c r="E79" s="83" t="n"/>
+      <c r="F79" s="83" t="n"/>
+      <c r="G79" s="83" t="n"/>
+      <c r="H79" s="83" t="n"/>
+      <c r="I79" s="83" t="n"/>
+    </row>
+    <row r="80">
+      <c r="C80" s="83" t="n"/>
+      <c r="D80" s="83" t="n"/>
+      <c r="E80" s="83" t="n"/>
+      <c r="F80" s="83" t="n"/>
+      <c r="G80" s="83" t="n"/>
+      <c r="H80" s="83" t="n"/>
+      <c r="I80" s="83" t="n"/>
+    </row>
+    <row r="81">
+      <c r="C81" s="83" t="n"/>
+      <c r="D81" s="83" t="n"/>
+      <c r="E81" s="83" t="n"/>
+      <c r="F81" s="83" t="n"/>
+      <c r="G81" s="83" t="n"/>
+      <c r="H81" s="83" t="n"/>
+      <c r="I81" s="83" t="n"/>
+    </row>
+    <row r="82">
+      <c r="C82" s="83" t="n"/>
+      <c r="D82" s="83" t="n"/>
+      <c r="E82" s="83" t="n"/>
+      <c r="F82" s="83" t="n"/>
+      <c r="G82" s="83" t="n"/>
+      <c r="H82" s="83" t="n"/>
+      <c r="I82" s="83" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.787401575" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.787401575"/>
@@ -948,8 +1528,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -967,8 +1547,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1953,7 +2533,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -1990,7 +2570,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -4134,7 +4714,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -4154,7 +4734,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -4243,7 +4823,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -4263,7 +4843,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -4407,7 +4987,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -5575,7 +6155,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -5610,7 +6190,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -5630,7 +6210,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -6413,7 +6993,7 @@
   <dimension ref="A2:Q163"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0" zoomScale="40" zoomScaleNormal="40">
-      <selection activeCell="I80" sqref="I80"/>
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -6431,8 +7011,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -7417,7 +7997,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -7454,7 +8034,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -9598,7 +10178,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -9618,7 +10198,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -9707,7 +10287,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -9727,7 +10307,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -9871,7 +10451,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -11039,7 +11619,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -11074,7 +11654,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -11094,7 +11674,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -11877,7 +12457,7 @@
   <dimension ref="A2:Q163"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0" zoomScale="55" zoomScaleNormal="55">
-      <selection activeCell="I80" sqref="I80"/>
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -11895,8 +12475,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -12881,7 +13461,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -12918,7 +13498,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -15062,7 +15642,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -15082,7 +15662,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -15171,7 +15751,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -15191,7 +15771,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -15335,7 +15915,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -16503,7 +17083,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -16538,7 +17118,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -16558,7 +17138,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -17340,8 +17920,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView topLeftCell="A25" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -17359,8 +17939,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -18345,7 +18925,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -18382,7 +18962,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -20526,7 +21106,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -20546,7 +21126,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -20635,7 +21215,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -20655,7 +21235,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -20799,7 +21379,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -21967,7 +22547,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -22002,7 +22582,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -22022,7 +22602,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -27706,8 +28286,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="B101" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView topLeftCell="B23" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -27725,8 +28305,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -28711,7 +29291,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -28748,7 +29328,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -30884,7 +31464,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -30904,7 +31484,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -30992,7 +31572,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -31012,7 +31592,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -31155,7 +31735,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -32315,7 +32895,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -32350,7 +32930,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -32370,7 +32950,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -32591,7 +33171,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -32614,7 +33194,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -32637,7 +33217,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -32660,7 +33240,7 @@
       </c>
       <c r="D135" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -32688,7 +33268,7 @@
       </c>
       <c r="D136" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -32716,7 +33296,7 @@
       </c>
       <c r="D137" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E137" s="82" t="inlineStr">
@@ -32744,7 +33324,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -32767,7 +33347,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -32790,7 +33370,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -32813,7 +33393,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -32869,7 +33449,7 @@
       </c>
       <c r="D143" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E143" s="82" t="inlineStr">
@@ -32897,7 +33477,7 @@
       </c>
       <c r="D144" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E144" s="82" t="inlineStr">
@@ -33152,8 +33732,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -33171,8 +33751,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -34157,7 +34737,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -34194,7 +34774,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -36338,7 +36918,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -36358,7 +36938,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -36447,7 +37027,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -36467,7 +37047,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -36611,7 +37191,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -37779,7 +38359,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -37814,7 +38394,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -37834,7 +38414,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -38055,7 +38635,7 @@
       </c>
       <c r="D132" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -38078,7 +38658,7 @@
       </c>
       <c r="D133" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -38101,7 +38681,7 @@
       </c>
       <c r="D134" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="82" t="inlineStr">
@@ -38208,7 +38788,7 @@
       </c>
       <c r="D138" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -38231,7 +38811,7 @@
       </c>
       <c r="D139" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -38254,7 +38834,7 @@
       </c>
       <c r="D140" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="82" t="inlineStr">
@@ -38277,7 +38857,7 @@
       </c>
       <c r="D141" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="82" t="inlineStr">
@@ -38616,8 +39196,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" workbookViewId="0" zoomScale="55" zoomScaleNormal="55">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView topLeftCell="A9" workbookViewId="0" zoomScale="55" zoomScaleNormal="55">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -38635,8 +39215,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -39621,7 +40201,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -39658,7 +40238,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -41802,7 +42382,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -41822,7 +42402,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -41911,7 +42491,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -41931,7 +42511,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -42075,7 +42655,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -43243,7 +43823,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -43278,7 +43858,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -43298,7 +43878,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -44080,8 +44660,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0" zoomScale="40" zoomScaleNormal="40">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView topLeftCell="A18" workbookViewId="0" zoomScale="40" zoomScaleNormal="40">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -44099,8 +44679,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -45085,7 +45665,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -45122,7 +45702,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -47266,7 +47846,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -47286,7 +47866,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -47375,7 +47955,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -47395,7 +47975,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -47539,7 +48119,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -48707,7 +49287,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -48742,7 +49322,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -48762,7 +49342,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -49052,7 +49632,7 @@
       </c>
       <c r="D135" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -49080,7 +49660,7 @@
       </c>
       <c r="D136" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -49108,7 +49688,7 @@
       </c>
       <c r="D137" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E137" s="82" t="inlineStr">
@@ -49261,7 +49841,7 @@
       </c>
       <c r="D143" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E143" s="82" t="inlineStr">
@@ -49289,7 +49869,7 @@
       </c>
       <c r="D144" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E144" s="82" t="inlineStr">
@@ -49545,8 +50125,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView topLeftCell="A25" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -49564,8 +50144,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -50550,7 +51130,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -50587,7 +51167,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -52731,7 +53311,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -52751,7 +53331,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -52840,7 +53420,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -52860,7 +53440,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -53004,7 +53584,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -54172,7 +54752,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -54207,7 +54787,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -54227,7 +54807,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -55010,7 +55590,7 @@
   <dimension ref="A2:Q163"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0" zoomScale="40" zoomScaleNormal="40">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -55028,8 +55608,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -56014,7 +56594,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -56051,7 +56631,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -58195,7 +58775,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -58215,7 +58795,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -58304,7 +58884,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -58324,7 +58904,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -58468,7 +59048,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -59636,7 +60216,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -59671,7 +60251,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -59691,7 +60271,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -60473,8 +61053,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0" zoomScale="109" zoomScaleNormal="109">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView topLeftCell="A26" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -60492,8 +61072,8 @@
     <col customWidth="1" max="12" min="12" style="74" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="74" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="74" width="90"/>
-    <col customWidth="1" max="46" min="15" style="74" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="47" style="74" width="10.6640625"/>
+    <col customWidth="1" max="49" min="15" style="74" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="50" style="74" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -61478,7 +62058,7 @@
       </c>
       <c r="G37" s="71" t="inlineStr">
         <is>
-          <t>[18:26)</t>
+          <t>[18:28)</t>
         </is>
       </c>
       <c r="H37" s="58" t="inlineStr">
@@ -61515,7 +62095,7 @@
       </c>
       <c r="G38" s="71" t="inlineStr">
         <is>
-          <t>[0,1,5,7,8,14,20]</t>
+          <t>[0,1,5,7,8,14,20,26,30]</t>
         </is>
       </c>
       <c r="H38" s="58" t="inlineStr">
@@ -63659,7 +64239,7 @@
       </c>
       <c r="E97" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F97" s="61" t="inlineStr">
@@ -63679,7 +64259,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+          <t>270df023-5a6b-456e-913e-296e51bcbdb7</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -63768,7 +64348,7 @@
       </c>
       <c r="E99" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F99" s="61" t="inlineStr">
@@ -63788,7 +64368,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+          <t>26720421-3b0c-4d6c-b3ca-010be568aa2e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -63932,7 +64512,7 @@
       </c>
       <c r="E102" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F102" s="61" t="inlineStr">
@@ -65100,7 +65680,7 @@
       </c>
       <c r="I123" s="52" t="inlineStr">
         <is>
-          <t>19d94eaa-249c-4713-8dc1-0ac501bb78a3</t>
+          <t>1cc15374-f6ec-410c-8ab1-c950b5be8533</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -65135,7 +65715,7 @@
       </c>
       <c r="E124" s="71" t="inlineStr">
         <is>
-          <t>V2.1</t>
+          <t>V2.2</t>
         </is>
       </c>
       <c r="F124" s="61" t="inlineStr">
@@ -65155,7 +65735,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>5a59c156-fbfa-4aec-aec9-0df4f6bc0b1c</t>
+          <t>a60de654-3183-4d5d-a602-cc722c5d8dbb</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -65445,7 +66025,7 @@
       </c>
       <c r="D135" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -65473,7 +66053,7 @@
       </c>
       <c r="D136" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -65501,7 +66081,7 @@
       </c>
       <c r="D137" s="71" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E137" s="82" t="inlineStr">

</xml_diff>